<commit_message>
izmijenjene vrijednosti u sabloni za uvezivanje
</commit_message>
<xml_diff>
--- a/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
+++ b/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesenovic/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesenovic/RubymineProjects/untitled1/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>email</t>
   </si>
@@ -91,15 +91,6 @@
     <t>01222</t>
   </si>
   <si>
-    <t>VIPNET d.o.o.</t>
-  </si>
-  <si>
-    <t>81793146560</t>
-  </si>
-  <si>
-    <t>Hrvatski Telekom d.d</t>
-  </si>
-  <si>
     <t>placeni_iznos_racuna</t>
   </si>
   <si>
@@ -134,6 +125,18 @@
   </si>
   <si>
     <t>broj_izdanog_racuna</t>
+  </si>
+  <si>
+    <t>Kompanija1 d.o.o.</t>
+  </si>
+  <si>
+    <t>Kompanija2 d.d</t>
+  </si>
+  <si>
+    <t>21111111114</t>
+  </si>
+  <si>
+    <t>81111111110</t>
   </si>
 </sst>
 </file>
@@ -498,25 +501,25 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -607,7 +610,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,24 +622,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>29524210204</v>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -644,10 +647,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +663,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,7 +678,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>8</v>
@@ -690,7 +693,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>12</v>
@@ -715,8 +718,8 @@
       <c r="F2" s="8">
         <v>1500</v>
       </c>
-      <c r="G2" s="3">
-        <v>29524210204</v>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -738,8 +741,8 @@
       <c r="F3" s="8">
         <v>2000.66</v>
       </c>
-      <c r="G3" s="3">
-        <v>29524210204</v>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -762,13 +765,10 @@
         <v>3200</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ispravljen dizajn izvjesca(ne prekida stranicu usred tablice)
</commit_message>
<xml_diff>
--- a/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
+++ b/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>email</t>
   </si>
@@ -88,9 +88,6 @@
     <t>broj</t>
   </si>
   <si>
-    <t>oznaka_poreznog_broja</t>
-  </si>
-  <si>
     <t>porezni_broj</t>
   </si>
   <si>
@@ -116,6 +113,12 @@
   </si>
   <si>
     <t>opz_ukupan_iznos_pdv</t>
+  </si>
+  <si>
+    <t>pdv_identifikacijski_broj</t>
+  </si>
+  <si>
+    <t>ostali_brojevi</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,10 +510,10 @@
         <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -561,50 +564,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -632,7 +633,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -673,7 +674,7 @@
         <v>1500</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -696,7 +697,7 @@
         <v>2000.66</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -719,7 +720,7 @@
         <v>3200</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
izradena funkcija za postavlanje 'nisu naplaceni do', 'datum od' i 'datum do' za uvezivanje excel tablice i kreiranje novog obrasca preko aplikacije
</commit_message>
<xml_diff>
--- a/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
+++ b/public/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <v>42653</v>
+        <v>42460</v>
       </c>
       <c r="H2" s="8">
         <v>0</v>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,10 +654,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>42470</v>
+        <v>42439</v>
       </c>
       <c r="C3" s="2">
-        <v>42470</v>
+        <v>42439</v>
       </c>
       <c r="D3" s="8">
         <v>20000.66</v>

</xml_diff>